<commit_message>
Xls + zmena vypoctu proudu
</commit_message>
<xml_diff>
--- a/openXsensor/Kalibrace.xlsx
+++ b/openXsensor/Kalibrace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\openXsensor\openXsensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127EBA6A-5196-4358-8392-CEB8CC345523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A5679-B3B8-4883-BB48-5514B88CF74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{C857F6EB-AD46-4AFE-9662-F52645D59401}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Senzor</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>INA139/XT60</t>
+  </si>
+  <si>
+    <t>60A</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3136482939632545E-2"/>
+          <c:y val="0.14757575757575758"/>
+          <c:w val="0.88386351706036748"/>
+          <c:h val="0.73901182806694621"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -644,10 +657,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.8</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105.3</c:v>
+                  <c:v>86.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,21 +936,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:backward val="1"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Proud!$A$10:$A$13</c:f>
@@ -966,16 +964,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.2</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.9</c:v>
+                  <c:v>63.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.3</c:v>
+                  <c:v>110.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,21 +1040,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:backward val="1"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Proud!$A$10:$A$13</c:f>
@@ -1084,17 +1067,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="0.000000">
-                  <c:v>0.4</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.8</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.8</c:v>
+                  <c:v>63.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>109.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1103,125 +1083,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-DF00-4FC7-BEF0-530D0B4871BA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:backward val="1"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Proud!$A$10:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0979999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Proud!$D$10:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>71.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>115.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-DF00-4FC7-BEF0-530D0B4871BA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3125,15 +2986,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3161,16 +3022,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3535,10 +3396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF82217D-3DE1-4022-AFBD-E042806667BF}">
-  <dimension ref="A3:D13"/>
+  <dimension ref="A3:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,7 +3408,7 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3555,84 +3416,108 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11.8</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>105.3</v>
+        <v>86.4</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.4</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2.8</v>
       </c>
+      <c r="F10">
+        <v>16.100000000000001</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
+        <v>13.8</v>
+      </c>
+      <c r="C11">
         <v>14.2</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>21.8</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>23.5</v>
       </c>
+      <c r="F11">
+        <v>29.8</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3.0979999999999999</v>
       </c>
       <c r="B12">
+        <v>63.7</v>
+      </c>
+      <c r="C12">
         <v>63.9</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>63.8</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>71.400000000000006</v>
       </c>
+      <c r="F12">
+        <v>59.2</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13">
+        <v>110.3</v>
+      </c>
+      <c r="C13">
         <v>109.3</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>100</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>115.9</v>
+      </c>
+      <c r="F13">
+        <v>87.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linearizace proudu pres krivku zacatek
</commit_message>
<xml_diff>
--- a/openXsensor/Kalibrace.xlsx
+++ b/openXsensor/Kalibrace.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\openXsensor\openXsensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A5679-B3B8-4883-BB48-5514B88CF74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4EC3DB-808D-4A27-8A2E-EB6AD5AC7150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{C857F6EB-AD46-4AFE-9662-F52645D59401}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{C857F6EB-AD46-4AFE-9662-F52645D59401}"/>
   </bookViews>
   <sheets>
     <sheet name="Napětí" sheetId="1" r:id="rId1"/>
-    <sheet name="Proud" sheetId="2" r:id="rId2"/>
+    <sheet name="Přehled" sheetId="2" r:id="rId2"/>
+    <sheet name="List1" sheetId="3" r:id="rId3"/>
+    <sheet name="List2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Senzor</t>
   </si>
@@ -43,19 +45,88 @@
     <t>Meřidlo</t>
   </si>
   <si>
-    <t>Měřidlo</t>
+    <t>R dolni</t>
   </si>
   <si>
-    <t>Sensor</t>
+    <t>R horni</t>
   </si>
   <si>
-    <t>INA139/4</t>
+    <t>Init</t>
   </si>
   <si>
-    <t>INA139/XT60</t>
+    <t>Kalibrace</t>
   </si>
   <si>
-    <t>60A</t>
+    <t>Bočník</t>
+  </si>
+  <si>
+    <t>Zesílení</t>
+  </si>
+  <si>
+    <t>napětí na amper</t>
+  </si>
+  <si>
+    <t>Proud nízký</t>
+  </si>
+  <si>
+    <t>Proud vysoký</t>
+  </si>
+  <si>
+    <t>Senzor nízký</t>
+  </si>
+  <si>
+    <t>Senzor vysoký</t>
+  </si>
+  <si>
+    <t>Koeficient</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Erik/01</t>
+  </si>
+  <si>
+    <t>Napětí LO</t>
+  </si>
+  <si>
+    <t>Snzor LO</t>
+  </si>
+  <si>
+    <t>Napětí HI</t>
+  </si>
+  <si>
+    <t>Snzor HI</t>
+  </si>
+  <si>
+    <t>Citabria</t>
+  </si>
+  <si>
+    <t>JET</t>
+  </si>
+  <si>
+    <t>ME110</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>R16;R20;R24;</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>RefVoltage[V]</t>
+  </si>
+  <si>
+    <t>fullRange[A]</t>
+  </si>
+  <si>
+    <t>mA/step</t>
   </si>
 </sst>
 </file>
@@ -63,9 +134,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,16 +145,68 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -91,16 +214,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Správně" xfId="1" builtinId="26"/>
+    <cellStyle name="Špatně" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -217,8 +417,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="10"/>
-            <c:backward val="10"/>
+            <c:backward val="1"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -259,10 +458,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.8320000000000007</c:v>
+                  <c:v>0.77700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.681999999999999</c:v>
+                  <c:v>4.0330000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,10 +473,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,17 +721,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.3136482939632545E-2"/>
-          <c:y val="0.14757575757575758"/>
-          <c:w val="0.88386351706036748"/>
-          <c:h val="0.73901182806694621"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -588,24 +777,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:backward val="1"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="#,##0.00000000" sourceLinked="0"/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -637,7 +813,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Proud!$B$4:$B$5</c:f>
+              <c:f>Přehled!$O$8:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -652,15 +828,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Proud!$A$4:$A$5</c:f>
+              <c:f>Přehled!$S$8:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>0.85299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86.4</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -668,7 +844,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D6D6-41B5-A7BF-18BD60E3AA4D}"/>
+              <c16:uniqueId val="{00000000-EF25-4D6E-A99F-20D9C9087487}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -680,11 +856,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1025506303"/>
-        <c:axId val="983125471"/>
+        <c:axId val="517615599"/>
+        <c:axId val="373009439"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1025506303"/>
+        <c:axId val="517615599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,12 +917,12 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="983125471"/>
+        <c:crossAx val="373009439"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="983125471"/>
+        <c:axId val="373009439"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +979,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1025506303"/>
+        <c:crossAx val="517615599"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -905,7 +1081,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5139629591329229E-2"/>
+          <c:y val="7.828544610731604E-2"/>
+          <c:w val="0.93344698704406792"/>
+          <c:h val="0.85845474613686534"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -936,9 +1122,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:forward val="1000"/>
+            <c:backward val="1000"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Proud!$A$10:$A$13</c:f>
+              <c:f>Přehled!$Q$18:$Q$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -946,34 +1149,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0979999999999999</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Proud!$B$10:$B$13</c:f>
+              <c:f>Přehled!$R$18:$R$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>853</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.7</c:v>
+                  <c:v>2785</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.3</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,108 +1184,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DF00-4FC7-BEF0-530D0B4871BA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Proud!$A$10:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0979999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Proud!$C$10:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="1">
-                  <c:v>14.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>63.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>109.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-DF00-4FC7-BEF0-530D0B4871BA}"/>
+              <c16:uniqueId val="{00000000-E967-417B-8284-0AF660B6DC73}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1094,11 +1196,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="9950960"/>
-        <c:axId val="7648096"/>
+        <c:axId val="1886480752"/>
+        <c:axId val="384668240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9950960"/>
+        <c:axId val="1886480752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,12 +1257,12 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7648096"/>
+        <c:crossAx val="384668240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7648096"/>
+        <c:axId val="384668240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1319,809 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9950960"/>
+        <c:crossAx val="1886480752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:backward val="1"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$F$4:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$H$4:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0173999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-93BA-4071-9F58-409FC613814C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$F$4:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$I$4:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-93BA-4071-9F58-409FC613814C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List1!$F$4:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List1!$J$4:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-93BA-4071-9F58-409FC613814C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="381222896"/>
+        <c:axId val="146445488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="381222896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146445488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146445488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="381222896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>List2!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>List2!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E88-45C3-88A3-8FCC517561FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="405296448"/>
+        <c:axId val="384060784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="405296448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="384060784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="384060784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405296448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1393,6 +2297,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2941,20 +3925,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2986,23 +5002,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>781051</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graf 2">
+        <xdr:cNvPr id="4" name="Graf 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E563946C-5529-43F2-BFA1-2BC76EFF2155}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B402897-051B-447D-9620-3FFA81F03145}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3022,23 +5038,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graf 1">
+        <xdr:cNvPr id="3" name="Graf 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90ED7B1D-BFCA-4B76-B29B-4D6EA8F7FAA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F87D8A2B-7E05-4473-B4C4-42BA5668BEAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3051,6 +5067,88 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7380C585-E01D-4D6B-813E-EA5D554FDEED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C64290A-ADD8-4C64-9E61-D3189CF76544}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3356,36 +5454,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4965ABF0-7A80-4B9E-ADA6-F9BE617AEF7A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9.8320000000000007</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>(B2-B3)/(A2-A3)</f>
+        <v>1.2285012285012284</v>
+      </c>
+      <c r="F2">
+        <v>3900</v>
+      </c>
+      <c r="G2">
+        <v>97600</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>19.681999999999999</v>
+        <v>4.0330000000000004</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f>B2-A2*D2</f>
+        <v>4.5454545454545414E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.CONCAT("V",F2,";W0;V",G2,";W4;V0.0;W8;V1.0;W12;")</f>
+        <v>V3900;W0;V97600;W4;V0.0;W8;V1.0;W12;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xlfn.CONCAT("V",D2,";W12;V",D3,";W8;")</f>
+        <v>V1.22850122850123;W12;V0.0454545454545454;W8;</v>
       </c>
     </row>
   </sheetData>
@@ -3396,128 +5536,605 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF82217D-3DE1-4022-AFBD-E042806667BF}">
-  <dimension ref="A3:F13"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="7.140625" style="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="7.28515625" style="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="9.5703125" style="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="8.5703125" style="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="9.140625" style="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.140625" style="11" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="9" width="16.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="38.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="48" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="3.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="7.7109375" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="15.42578125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="13.7109375" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="12.140625" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="12" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="11.140625" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="11.85546875" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="15.85546875" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="13.5703125" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="10.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="14.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="37.7109375" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="48.42578125" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="12" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:27" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="D1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>27</v>
-      </c>
-      <c r="B4">
+    <row r="2" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="10">
+        <v>3900</v>
+      </c>
+      <c r="C2" s="10">
+        <v>97600</v>
+      </c>
+      <c r="D2" s="10">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10.186</v>
+      </c>
+      <c r="F2" s="10">
+        <v>25</v>
+      </c>
+      <c r="G2" s="10">
+        <v>25.533000000000001</v>
+      </c>
+      <c r="H2" s="8">
+        <f>(D2-F2)/(E2-G2)</f>
+        <v>0.97738971786016804</v>
+      </c>
+      <c r="I2" s="8">
+        <f>D2-E2*H2</f>
+        <v>4.4308333876328376E-2</v>
+      </c>
+      <c r="J2" s="8" t="str">
+        <f>_xlfn.CONCAT("V",B2,";W0;V",C2,";W4;V0.0;W8;V1.0;W12;")</f>
+        <v>V3900;W0;V97600;W4;V0.0;W8;V1.0;W12;</v>
+      </c>
+      <c r="K2" s="8" t="str">
+        <f>_xlfn.CONCAT("V",H2,";W12;V",I2,";W8;")</f>
+        <v>V0.977389717860168;W12;V0.0443083338763284;W8;</v>
+      </c>
+      <c r="M2" s="10">
+        <v>3.5E-4</v>
+      </c>
+      <c r="N2" s="10">
+        <v>50</v>
+      </c>
+      <c r="O2" s="8">
+        <f>M2*1*N2</f>
+        <v>1.7499999999999998E-2</v>
+      </c>
+      <c r="S2" s="10">
         <v>1</v>
       </c>
+      <c r="T2" s="10">
+        <v>1.5980000000000001</v>
+      </c>
+      <c r="U2" s="10">
+        <v>5</v>
+      </c>
+      <c r="V2" s="10">
+        <v>4.97</v>
+      </c>
+      <c r="W2" s="9">
+        <f>(T2-V2)/(S2-U2)</f>
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="X2" s="9">
+        <f>T2-S2*W2/(1/W2)</f>
+        <v>0.88735100000000011</v>
+      </c>
+      <c r="Y2" s="8" t="str">
+        <f>_xlfn.CONCAT("V0;W16;V",O2*1000,";W20; V1;W24;")</f>
+        <v>V0;W16;V17.5;W20; V1;W24;</v>
+      </c>
+      <c r="Z2" s="8" t="str">
+        <f>_xlfn.CONCAT("V",X2,";W16; V",1/W2,";W24;")</f>
+        <v>V0.887351;W16; V1.18623962040332;W24;</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>86.4</v>
-      </c>
-      <c r="B5">
+    <row r="3" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="14">
+        <v>5100</v>
+      </c>
+      <c r="C3" s="14">
+        <v>97600</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14">
+        <v>9.8420000000000005</v>
+      </c>
+      <c r="F3" s="14">
+        <v>20</v>
+      </c>
+      <c r="G3" s="14">
+        <v>19.7</v>
+      </c>
+      <c r="H3" s="14">
+        <f>(D3-F3)/(E3-G3)</f>
+        <v>1.0144045445323597</v>
+      </c>
+      <c r="I3" s="14">
+        <f>D3-E3*H3</f>
+        <v>1.6230472712514654E-2</v>
+      </c>
+      <c r="J3" s="14" t="str">
+        <f>_xlfn.CONCAT("V",B3,";W0;V",C3,";W4;V0.0;W8;V1.0;W12;")</f>
+        <v>V5100;W0;V97600;W4;V0.0;W8;V1.0;W12;</v>
+      </c>
+      <c r="K3" s="14" t="str">
+        <f>_xlfn.CONCAT("V",H3,";W12;V",I3,";W8;")</f>
+        <v>V1.01440454453236;W12;V0.0162304727125147;W8;</v>
+      </c>
+      <c r="M3" s="14">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="N3" s="14">
+        <v>50</v>
+      </c>
+      <c r="O3" s="14">
+        <f>M3*1*N3</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S3" s="14">
+        <v>1</v>
+      </c>
+      <c r="T3" s="14">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="U3" s="14">
         <v>5</v>
       </c>
+      <c r="V3" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="W3" s="15">
+        <f>(S3-U3)/(T3-V3)</f>
+        <v>1.0967918837400603</v>
+      </c>
+      <c r="X3" s="14">
+        <f>(T3-S3*(1/W3))*W3</f>
+        <v>-6.4436523169728629E-2</v>
+      </c>
+      <c r="Y3" s="14" t="str">
+        <f t="shared" ref="Y3" si="0">_xlfn.CONCAT("V0;W16;V",O3*1000,";W20; V1;W24;")</f>
+        <v>V0;W16;V25;W20; V1;W24;</v>
+      </c>
+      <c r="Z3" s="14" t="str">
+        <f>_xlfn.CONCAT("V",X3,";W16; V",W3,";W24;")</f>
+        <v>V-0.0644365231697286;W16; V1.09679188374006;W24;</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="11">
+        <v>5100</v>
+      </c>
+      <c r="C4" s="11">
+        <v>97600</v>
+      </c>
+      <c r="D4" s="11">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11">
+        <v>19.7</v>
+      </c>
+      <c r="F4" s="11">
+        <v>20</v>
+      </c>
+      <c r="G4" s="11">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H5" si="1">(D4-F4)/(E4-G4)</f>
+        <v>4.3478260869565206</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I5" si="2">D4-E4*H4</f>
+        <v>-75.652173913043455</v>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f t="shared" ref="J4:J5" si="3">_xlfn.CONCAT("V",B4,";W0;V",C4,";W4;V0.0;W8;V1.0;W12;")</f>
+        <v>V5100;W0;V97600;W4;V0.0;W8;V1.0;W12;</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f t="shared" ref="K4:K5" si="4">_xlfn.CONCAT("V",H4,";W12;V",I4,";W8;")</f>
+        <v>V4.34782608695652;W12;V-75.6521739130435;W8;</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="N4" s="11">
+        <v>50</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O5" si="5">M4*1*N4</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>P4/O4</f>
+        <v>44</v>
+      </c>
+      <c r="R4" s="2">
+        <f>Q4/1023*1000</f>
+        <v>43.010752688172047</v>
+      </c>
+      <c r="S4" s="11">
+        <v>1</v>
+      </c>
+      <c r="T4" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="U4" s="1">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>6</v>
+      <c r="V4" s="1">
+        <v>4.58</v>
+      </c>
+      <c r="W4" s="1">
+        <f>(T4-V4)/(S4-U4)</f>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="X4" s="1">
+        <f>(T4-S4*(W4))*1</f>
+        <v>-9.5000000000000084E-2</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f>_xlfn.CONCAT("V0;W16;V",R4,";W20; V1;W24;")</f>
+        <v>V0;W16;V43.010752688172;W20; V1;W24;</v>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <f>_xlfn.CONCAT("V",X4,";W16; V",W4,";W24;")</f>
+        <v>V-0.0950000000000001;W16; V0.935;W24;</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="11">
+        <v>5100</v>
+      </c>
+      <c r="C5" s="11">
+        <v>97600</v>
+      </c>
+      <c r="D5" s="11">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11">
+        <v>13.5</v>
+      </c>
+      <c r="F5" s="11">
+        <v>20</v>
+      </c>
+      <c r="G5" s="11">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.2105263157894726</v>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>V5100;W0;V97600;W4;V0.0;W8;V1.0;W12;</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>V1.05263157894737;W12;V-4.21052631578947;W8;</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="N5" s="11">
+        <v>50</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="11">
+        <v>1</v>
+      </c>
+      <c r="U5" s="11">
+        <v>5</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W7" s="11">
+        <f>1/W4</f>
+        <v>1.0695187165775399</v>
+      </c>
+      <c r="X7" s="11">
+        <f>1/X4</f>
+        <v>-10.526315789473674</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O8" s="1">
+        <v>1</v>
+      </c>
+      <c r="S8" s="11">
+        <f>T3</f>
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="T8" s="11">
+        <f>O8-S8</f>
+        <v>0.14700000000000002</v>
+      </c>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O9" s="1">
+        <v>5</v>
+      </c>
+      <c r="S9" s="11">
+        <f>V3</f>
+        <v>4.5</v>
+      </c>
+      <c r="T9" s="11">
+        <f>O9-S9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O12" s="1">
+        <f>1/(O3*W3)</f>
+        <v>36.47</v>
+      </c>
+      <c r="T12" s="11">
+        <f>-0.12/X3</f>
+        <v>1.8622978723404231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="T13" s="11">
+        <f>O12/T12</f>
+        <v>19.583333333333357</v>
+      </c>
+    </row>
+    <row r="17" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>1</v>
+      </c>
+      <c r="R17" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O18" s="11">
         <v>0</v>
       </c>
-      <c r="B10">
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E10">
-        <v>2.8</v>
-      </c>
-      <c r="F10">
-        <v>16.100000000000001</v>
+      <c r="P18" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="11">
+        <f>O18/Q$17</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
+        <f>P18*R$17</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>13.8</v>
-      </c>
-      <c r="C11">
-        <v>14.2</v>
-      </c>
-      <c r="D11">
-        <v>21.8</v>
-      </c>
-      <c r="E11">
-        <v>23.5</v>
-      </c>
-      <c r="F11">
-        <v>29.8</v>
-      </c>
+    <row r="19" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O19" s="11">
+        <v>1000</v>
+      </c>
+      <c r="P19" s="11">
+        <v>853</v>
+      </c>
+      <c r="Q19" s="11">
+        <f>O19/Q$17</f>
+        <v>1000</v>
+      </c>
+      <c r="R19" s="11">
+        <f>P19*R$17</f>
+        <v>853</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3.0979999999999999</v>
-      </c>
-      <c r="B12">
-        <v>63.7</v>
-      </c>
-      <c r="C12">
-        <v>63.9</v>
-      </c>
-      <c r="D12">
-        <v>63.8</v>
-      </c>
-      <c r="E12">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="F12">
-        <v>59.2</v>
-      </c>
+    <row r="20" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O20" s="11">
+        <v>3100</v>
+      </c>
+      <c r="P20" s="11">
+        <v>2785</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>3100</v>
+      </c>
+      <c r="R20" s="11">
+        <f>P20*R$17</f>
+        <v>2785</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>110.3</v>
-      </c>
-      <c r="C13">
-        <v>109.3</v>
-      </c>
-      <c r="D13">
-        <v>100</v>
-      </c>
-      <c r="E13">
-        <v>115.9</v>
-      </c>
-      <c r="F13">
-        <v>87.4</v>
+    <row r="21" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O21" s="11">
+        <v>5000</v>
+      </c>
+      <c r="P21" s="11">
+        <v>4500</v>
+      </c>
+      <c r="Q21" s="11">
+        <f>O21/Q$17</f>
+        <v>5000</v>
+      </c>
+      <c r="R21" s="11">
+        <f>P21*R$17</f>
+        <v>4500</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+    </row>
+    <row r="23" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="U23" s="11">
+        <f>77.5/50</f>
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="24" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O24" s="1">
+        <v>1023</v>
+      </c>
+      <c r="S24" s="11">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="25" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O25" s="1">
+        <v>2500</v>
+      </c>
+      <c r="S25" s="11">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="27" spans="15:21" x14ac:dyDescent="0.25">
+      <c r="O27" s="11">
+        <f>O25/O24</f>
+        <v>2.4437927663734116</v>
+      </c>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11">
+        <f>S25/S24</f>
+        <v>1.075268817204301</v>
       </c>
     </row>
   </sheetData>
@@ -3525,4 +6142,216 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2230C05E-47F1-4AB0-A1C2-173514647344}">
+  <dimension ref="B1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1.9E-3</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <f>B3*F$2</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>C3*G$2</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="H3">
+        <f>D3*H$2+H$1</f>
+        <v>0.1023</v>
+      </c>
+      <c r="I3">
+        <f>E3*I$2</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>22.5</v>
+      </c>
+      <c r="D4">
+        <v>19.5</v>
+      </c>
+      <c r="E4">
+        <v>850</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F5" si="0">B4*F$2</f>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G5" si="1">C4*G$2</f>
+        <v>22.5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H5" si="2">D4*H$2+H$1</f>
+        <v>0.997</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="H4:I5" si="3">E4*I$2</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J5" si="4">F4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>116.3</v>
+      </c>
+      <c r="D5">
+        <v>106.9</v>
+      </c>
+      <c r="E5">
+        <v>4610</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>116.3</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>5.0173999999999994</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BE4EFB-0D27-4E23-91F0-EBEDA763D1F8}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1.4</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>19.5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>107</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>107/5*C6</f>
+        <v>642</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>107/5*C7</f>
+        <v>856</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>107/5*C8</f>
+        <v>1022.9199999999998</v>
+      </c>
+      <c r="C8">
+        <v>47.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>